<commit_message>
FIxed all graph issues
</commit_message>
<xml_diff>
--- a/Test_Data.xlsx
+++ b/Test_Data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>File Name</t>
   </si>
@@ -55,19 +55,22 @@
     <t>positive</t>
   </si>
   <si>
+    <t>ovvertiode</t>
+  </si>
+  <si>
+    <t>2024.1.2</t>
+  </si>
+  <si>
+    <t>test login page</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
     <t>test</t>
-  </si>
-  <si>
-    <t>2024.1.2</t>
-  </si>
-  <si>
-    <t>test login page</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>low</t>
   </si>
   <si>
     <t>test login page22</t>
@@ -555,7 +558,7 @@
         <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
         <v>15</v>
@@ -566,10 +569,10 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -581,7 +584,7 @@
         <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H4" t="s">
         <v>17</v>
@@ -589,19 +592,19 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -615,16 +618,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
added support for more tags
</commit_message>
<xml_diff>
--- a/Test_Data.xlsx
+++ b/Test_Data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>File Name</t>
   </si>
@@ -37,6 +37,12 @@
     <t>Sprint</t>
   </si>
   <si>
+    <t>User Story</t>
+  </si>
+  <si>
+    <t>Test Case ID</t>
+  </si>
+  <si>
     <t>login.spec.ts</t>
   </si>
   <si>
@@ -61,7 +67,13 @@
     <t>2024.1.2</t>
   </si>
   <si>
-    <t>test login page</t>
+    <t>https://jira.app.syfbank.com/browse/SAK-1over</t>
+  </si>
+  <si>
+    <t>666</t>
+  </si>
+  <si>
+    <t>login page</t>
   </si>
   <si>
     <t/>
@@ -73,13 +85,10 @@
     <t>test</t>
   </si>
   <si>
-    <t>test login page22</t>
-  </si>
-  <si>
-    <t>page22</t>
-  </si>
-  <si>
-    <t>ace</t>
+    <t>https://jira.app.syfbank.com/browse/SAK-143</t>
+  </si>
+  <si>
+    <t>777</t>
   </si>
   <si>
     <t>addProductToCart.spec.ts</t>
@@ -92,6 +101,12 @@
   </si>
   <si>
     <t>medium</t>
+  </si>
+  <si>
+    <t>https://jira.app.syfbank.com/browse/SAK-123</t>
+  </si>
+  <si>
+    <t>1234</t>
   </si>
   <si>
     <t>reqres.spec.ts</t>
@@ -477,16 +492,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:J5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="50" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
     <col min="4" max="8" width="15" customWidth="1"/>
+    <col min="9" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -511,135 +527,139 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" t="s">
         <v>15</v>
       </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="I5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>